<commit_message>
updated DPPDTT dataset copy
</commit_message>
<xml_diff>
--- a/controlled_vocabulary.xlsx
+++ b/controlled_vocabulary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\GitHub\ofet-db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\GitHub\ofet-db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925301A7-9BD3-49FA-A469-EBD152E83CE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B0E1DB-127B-4282-899F-A74C9F67294A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main_table_features" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>sidechain</t>
   </si>
   <si>
-    <t>If not synthesized, the company name of the supplier. Ex.) Rieke Metals</t>
-  </si>
-  <si>
     <t>Batch identifier number, if vendor provided</t>
   </si>
   <si>
@@ -647,9 +644,6 @@
     <t>inkjet</t>
   </si>
   <si>
-    <t>wire_bar</t>
-  </si>
-  <si>
     <t>dip</t>
   </si>
   <si>
@@ -840,6 +834,12 @@
   </si>
   <si>
     <t>Preferred name from IUPAC. Listed under "IUPAC Name" in PubChem. Note that CRIPT vocab has "preferred_name"</t>
+  </si>
+  <si>
+    <t>If not synthesized in-house, the company name of the supplier. Ex.) Rieke Metals</t>
+  </si>
+  <si>
+    <t>wire</t>
   </si>
 </sst>
 </file>
@@ -1214,22 +1214,22 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="105.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" customWidth="1"/>
+    <col min="5" max="5" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="6" customFormat="1" ht="19.5" thickBot="1">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1249,10 +1249,10 @@
         <v>11</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" ht="15.75" thickTop="1"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="15" thickTop="1"/>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>9</v>
@@ -1290,7 +1290,7 @@
         <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1310,7 +1310,7 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1330,7 +1330,7 @@
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1350,7 +1350,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1370,7 +1370,7 @@
         <v>12</v>
       </c>
       <c r="G8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1390,7 +1390,7 @@
         <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1410,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1"/>
@@ -1454,10 +1454,10 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D15" t="s">
         <v>32</v>
@@ -1494,7 +1494,7 @@
         <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
@@ -1506,7 +1506,7 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
@@ -1585,13 +1585,13 @@
         <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>265</v>
       </c>
       <c r="F25" t="s">
         <v>12</v>
       </c>
       <c r="G25" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1602,13 +1602,13 @@
         <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1619,19 +1619,19 @@
         <v>56</v>
       </c>
       <c r="C27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D27" t="s">
         <v>60</v>
       </c>
-      <c r="D27" t="s">
-        <v>61</v>
-      </c>
       <c r="E27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1642,25 +1642,25 @@
         <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F28" t="s">
         <v>12</v>
       </c>
       <c r="G28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="4" customFormat="1"/>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
         <v>65</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>66</v>
-      </c>
-      <c r="C30" t="s">
-        <v>67</v>
       </c>
       <c r="E30" t="s">
         <v>41</v>
@@ -1672,16 +1672,16 @@
     <row r="31" spans="1:7" s="3" customFormat="1"/>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" t="s">
         <v>68</v>
       </c>
-      <c r="C32" t="s">
-        <v>69</v>
-      </c>
       <c r="E32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F32" t="s">
         <v>12</v>
@@ -1689,53 +1689,53 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F33" t="s">
         <v>12</v>
       </c>
       <c r="G33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B34" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
         <v>33</v>
       </c>
       <c r="G34" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>38</v>
@@ -1744,116 +1744,116 @@
         <v>33</v>
       </c>
       <c r="G35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
       </c>
       <c r="G36" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F37" t="s">
         <v>34</v>
       </c>
       <c r="G37" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" t="s">
         <v>34</v>
       </c>
       <c r="G38" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
         <v>154</v>
       </c>
-      <c r="B39" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" t="s">
-        <v>155</v>
-      </c>
       <c r="D39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F39" t="s">
         <v>34</v>
       </c>
       <c r="G39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:7" s="4" customFormat="1"/>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F41" t="s">
         <v>33</v>
       </c>
       <c r="G41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C42" t="s">
         <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>82</v>
       </c>
       <c r="E42" t="s">
         <v>41</v>
@@ -1862,452 +1862,452 @@
         <v>34</v>
       </c>
       <c r="G42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F43" t="s">
         <v>12</v>
       </c>
       <c r="G43" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:7" s="4" customFormat="1"/>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
         <v>96</v>
       </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
       <c r="C45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" t="s">
         <v>106</v>
-      </c>
-      <c r="E45" t="s">
-        <v>107</v>
       </c>
       <c r="F45" t="s">
         <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F46" t="s">
         <v>34</v>
       </c>
       <c r="G46" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F47" t="s">
         <v>34</v>
       </c>
       <c r="G47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E48" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F48" t="s">
         <v>12</v>
       </c>
       <c r="G48" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E49" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F49" t="s">
         <v>12</v>
       </c>
       <c r="G49" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F50" t="s">
         <v>12</v>
       </c>
       <c r="G50" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
         <v>34</v>
       </c>
       <c r="G52" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B53" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D53" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F53" t="s">
         <v>34</v>
       </c>
       <c r="G53" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="54" spans="1:7" s="4" customFormat="1"/>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
         <v>121</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>122</v>
       </c>
-      <c r="C55" t="s">
+      <c r="E55" t="s">
         <v>123</v>
-      </c>
-      <c r="E55" t="s">
-        <v>124</v>
       </c>
       <c r="F55" t="s">
         <v>12</v>
       </c>
       <c r="G55" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F56" t="s">
         <v>34</v>
       </c>
       <c r="G56" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D57" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F57" t="s">
         <v>34</v>
       </c>
       <c r="G57" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" t="s">
         <v>129</v>
       </c>
-      <c r="C58" t="s">
+      <c r="E58" t="s">
         <v>130</v>
-      </c>
-      <c r="E58" t="s">
-        <v>131</v>
       </c>
       <c r="F58" t="s">
         <v>12</v>
       </c>
       <c r="G58" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C59" t="s">
         <v>133</v>
       </c>
-      <c r="C59" t="s">
-        <v>134</v>
-      </c>
       <c r="D59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F59" t="s">
         <v>34</v>
       </c>
       <c r="G59" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F60" t="s">
         <v>34</v>
       </c>
       <c r="G60" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F61" t="s">
         <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F62" t="s">
         <v>34</v>
       </c>
       <c r="G62" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C63" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F63" t="s">
         <v>34</v>
       </c>
       <c r="G63" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F64" t="s">
         <v>34</v>
       </c>
       <c r="G64" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F66" t="s">
         <v>34</v>
       </c>
       <c r="G66" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="3" customFormat="1"/>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" t="s">
         <v>156</v>
       </c>
-      <c r="B68" t="s">
-        <v>157</v>
-      </c>
       <c r="C68" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E68" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
@@ -2315,144 +2315,144 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B69" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C69" t="s">
+        <v>169</v>
+      </c>
+      <c r="E69" t="s">
         <v>170</v>
-      </c>
-      <c r="E69" t="s">
-        <v>171</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B70" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C70" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D70" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F70" t="s">
         <v>34</v>
       </c>
       <c r="G70" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C71" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F71" t="s">
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C72" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D72" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F72" t="s">
         <v>34</v>
       </c>
       <c r="G72" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C73" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F73" t="s">
         <v>34</v>
       </c>
       <c r="G73" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B74" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F74" t="s">
         <v>34</v>
       </c>
       <c r="G74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B75" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F75" t="s">
         <v>12</v>
       </c>
       <c r="G75" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B76" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>38</v>
@@ -2461,61 +2461,61 @@
         <v>34</v>
       </c>
       <c r="G76" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F77" t="s">
         <v>33</v>
       </c>
       <c r="G77" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C78" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D78" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F78" t="s">
         <v>33</v>
       </c>
       <c r="G78" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C79" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F79" t="s">
         <v>12</v>
       </c>
       <c r="G79" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -2529,19 +2529,19 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="19.5" thickBot="1">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2550,181 +2550,181 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1">
+    <row r="2" spans="1:3" ht="15" thickTop="1">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="4" customFormat="1"/>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B13" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>266</v>
       </c>
       <c r="C16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="4" customFormat="1"/>
@@ -2741,16 +2741,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1">
+    <row r="1" spans="1:3" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -2759,103 +2759,103 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1">
+    <row r="2" spans="1:3" ht="15" thickTop="1">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C3" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B7" t="s">
+        <v>256</v>
+      </c>
+      <c r="C7" t="s">
         <v>258</v>
-      </c>
-      <c r="C7" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" t="s">
         <v>259</v>
-      </c>
-      <c r="C8" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2868,19 +2868,19 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" ht="19.5" thickBot="1">
+    <row r="1" spans="1:6" s="6" customFormat="1" ht="18.600000000000001" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -2897,67 +2897,67 @@
         <v>11</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickTop="1">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1"/>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D9" t="s">
         <v>41</v>
@@ -2966,162 +2966,162 @@
     <row r="10" spans="1:6" s="4" customFormat="1"/>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B12" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B13" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="4" customFormat="1"/>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B20" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B21" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C21" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1"/>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B28" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>